<commit_message>
Added Template for latex
</commit_message>
<xml_diff>
--- a/Lars/user_cases_and_requirements.xlsx
+++ b/Lars/user_cases_and_requirements.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larsf\Desktop\swea-team5group6\Lars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7408ED8F-B333-4E9C-988E-CC9565A6EEC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08568BD0-05AE-44E2-9C06-359593211DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="3" activeTab="4" xr2:uid="{A4EC47FB-7C6E-4723-8829-476AF0E84542}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" firstSheet="3" activeTab="6" xr2:uid="{A4EC47FB-7C6E-4723-8829-476AF0E84542}"/>
   </bookViews>
   <sheets>
     <sheet name="#1 Browsing for file" sheetId="1" r:id="rId1"/>
     <sheet name="#2 Specify delimiter" sheetId="3" r:id="rId2"/>
     <sheet name="#3 Select file" sheetId="2" r:id="rId3"/>
     <sheet name="Sleep Analysis" sheetId="7" r:id="rId4"/>
-    <sheet name="Virtual Assistant Web" sheetId="8" r:id="rId5"/>
+    <sheet name="Focus Manager" sheetId="10" r:id="rId5"/>
+    <sheet name="Virtual Assistant Web" sheetId="8" r:id="rId6"/>
+    <sheet name="Gesture Control" sheetId="9" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'#1 Browsing for file'!$A$1:$D$18</definedName>
@@ -25,7 +27,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">'#3 Select file'!$A$1:$D$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="121">
   <si>
     <t>Name</t>
   </si>
@@ -229,19 +230,10 @@
     <t>The system summarises the retreived information using a free online AI tool</t>
   </si>
   <si>
-    <t>The system returns the information by reading the summary out loud</t>
-  </si>
-  <si>
     <t>Requirement</t>
   </si>
   <si>
     <t>User get got information he wanted witohout having to pull out phone or moving hand</t>
-  </si>
-  <si>
-    <t>A user must be able to quickly access information from the web.
-This cant be done on a tiny smartwatch display, which is
- why a virtual voice directed assistent needs to be implemented.
-The feature would allow for hands free easy data retrerival.</t>
   </si>
   <si>
     <t>The smartwatch is not connected to the internet</t>
@@ -265,6 +257,150 @@
     <t>A user must be able to quickly access information from the web while not being able to acces smartphone. This cant be done on a tiny smartwatch display, which is
 why a virtual voice directed assistent needs to be implemented.
 The feature would allow for hands free easy data retrerival.</t>
+  </si>
+  <si>
+    <t>Monitor and display sleep patterns and quality</t>
+  </si>
+  <si>
+    <t>Show sleeping pattern chart and score of sleeping quality</t>
+  </si>
+  <si>
+    <t>Set a goal of sleeping time, and system is notified that user's heart rate patter is changed to sleeping pattern from heart rate sensor.</t>
+  </si>
+  <si>
+    <t>User, Sleeping system</t>
+  </si>
+  <si>
+    <t>Smartwatch turned on, Sleep monitoring app opened</t>
+  </si>
+  <si>
+    <t>User get information about their last sleep</t>
+  </si>
+  <si>
+    <t>This is the main scenario when the heart rate system works</t>
+  </si>
+  <si>
+    <t>The user refresh the monitor of sleeping app</t>
+  </si>
+  <si>
+    <t>The system notices user starts to sleep and therefore starts to record heartbeat</t>
+  </si>
+  <si>
+    <t>The system notices user wakes up and stops heart beta recording</t>
+  </si>
+  <si>
+    <t>The system calculates sleep quality (score between 0 and 100)</t>
+  </si>
+  <si>
+    <t>The system shows the quality score on the app</t>
+  </si>
+  <si>
+    <t>User, System, Gyroscope Sensor</t>
+  </si>
+  <si>
+    <t>Smartwatch is turned on</t>
+  </si>
+  <si>
+    <t>This is the main scenario where the system recognizes the hand up movement</t>
+  </si>
+  <si>
+    <t>User raises arm</t>
+  </si>
+  <si>
+    <t>System recognizes gesture</t>
+  </si>
+  <si>
+    <t>Display turns on</t>
+  </si>
+  <si>
+    <t>The system recognizes hand down movement</t>
+  </si>
+  <si>
+    <t>User lowers arm</t>
+  </si>
+  <si>
+    <t>Display turns off</t>
+  </si>
+  <si>
+    <t>The system recognizes other motion</t>
+  </si>
+  <si>
+    <t>User moves arm</t>
+  </si>
+  <si>
+    <t>System doesnt recognize any gesture</t>
+  </si>
+  <si>
+    <t>Use gestures to execute actions on smartwatch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display on/off, App opened, </t>
+  </si>
+  <si>
+    <t>When the user lifts his arm and turns his wrist the smartwatch display turns on, when he lowers the arm the display turns of. Additionally the smartwatch executes a costum gesture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User lifting/lowering arm and turning wrist, or the </t>
+  </si>
+  <si>
+    <t>Click "Start working session"</t>
+  </si>
+  <si>
+    <t>Smartwatch turned on, Bluetooth on</t>
+  </si>
+  <si>
+    <t>User had a productive working session</t>
+  </si>
+  <si>
+    <t>User, System, Smartphone</t>
+  </si>
+  <si>
+    <t>User selects number of "work cycles"</t>
+  </si>
+  <si>
+    <t>Button "Start working session" appears</t>
+  </si>
+  <si>
+    <t>User clicks the button</t>
+  </si>
+  <si>
+    <t>User works until break starts</t>
+  </si>
+  <si>
+    <t>User starts working again</t>
+  </si>
+  <si>
+    <t>This is the main scenario where the user starts a working session with just 1 work cycle</t>
+  </si>
+  <si>
+    <t>The smartwatch ends the working session</t>
+  </si>
+  <si>
+    <t>The User tries to use his phone during the working session</t>
+  </si>
+  <si>
+    <t>The user ends the work cycle prematurely</t>
+  </si>
+  <si>
+    <t>The user taps on button "End work cycle"</t>
+  </si>
+  <si>
+    <t>The system notices the user takes out phone</t>
+  </si>
+  <si>
+    <t>The Smartwatch vibrates to remind user to stay on track, and prevents phone usage</t>
+  </si>
+  <si>
+    <t>The smartwatch doesnt count this work cycle.</t>
+  </si>
+  <si>
+    <t>Requriement for productivity feature: when focus mode activated, user is reminden that he should work when the system recognizes he does something else.</t>
+  </si>
+  <si>
+    <t>Use smartwatch to stay off phone and keep focus on work.</t>
+  </si>
+  <si>
+    <t>Smartwatch reminds you to stay on track with work, by vibrating when you try to look at your phone or try to do something else while working. You can decide on how many "work cycles" you want to do. Each work cycle is 30m work and 5m break and then another 30min work.</t>
   </si>
 </sst>
 </file>
@@ -326,7 +462,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -689,12 +825,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -813,13 +984,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -827,21 +991,17 @@
     <xf numFmtId="16" fontId="3" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -855,6 +1015,36 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1708,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D56253-CCB1-4A3B-81FC-1F410907DB03}">
   <dimension ref="A1:K104"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1720,11 +1910,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="56" t="s">
-        <v>67</v>
+      <c r="A1" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28" t="s">
+        <v>73</v>
       </c>
       <c r="E1" s="29"/>
       <c r="F1" s="29"/>
@@ -1735,6 +1927,14 @@
       <c r="K1" s="29"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33">
+        <v>4</v>
+      </c>
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
@@ -1744,6 +1944,14 @@
       <c r="K2" s="29"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="65"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="E3" s="29"/>
       <c r="F3" s="29"/>
       <c r="G3" s="29"/>
@@ -1752,14 +1960,14 @@
       <c r="J3" s="29"/>
       <c r="K3" s="29"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A4" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="28" t="s">
-        <v>53</v>
+    <row r="4" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="35" t="s">
+        <v>75</v>
       </c>
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
@@ -1771,12 +1979,12 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="30" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5" s="31"/>
       <c r="C5" s="32"/>
-      <c r="D5" s="33">
-        <v>0</v>
+      <c r="D5" s="35" t="s">
+        <v>76</v>
       </c>
       <c r="E5" s="29"/>
       <c r="F5" s="29"/>
@@ -1787,13 +1995,13 @@
       <c r="K5" s="29"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" s="52" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="53"/>
+      <c r="A6" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="65"/>
       <c r="C6" s="32"/>
       <c r="D6" s="35" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="E6" s="29"/>
       <c r="F6" s="29"/>
@@ -1804,13 +2012,13 @@
       <c r="K6" s="29"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A7" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="32"/>
+      <c r="A7" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="65"/>
+      <c r="C7" s="66"/>
       <c r="D7" s="35" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
@@ -1821,14 +2029,12 @@
       <c r="K7" s="29"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A8" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="35" t="s">
-        <v>56</v>
-      </c>
+      <c r="A8" s="67" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="68"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="29"/>
       <c r="F8" s="29"/>
       <c r="G8" s="29"/>
@@ -1838,13 +2044,13 @@
       <c r="K8" s="29"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A9" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="35" t="s">
-        <v>57</v>
+      <c r="A9" s="41"/>
+      <c r="B9" s="69" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="70"/>
+      <c r="D9" s="40" t="s">
+        <v>79</v>
       </c>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
@@ -1855,14 +2061,12 @@
       <c r="K9" s="29"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A10" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="35" t="s">
-        <v>66</v>
-      </c>
+      <c r="A10" s="41"/>
+      <c r="B10" s="69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="70"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
       <c r="G10" s="29"/>
@@ -1872,12 +2076,14 @@
       <c r="K10" s="29"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="40"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="44">
+        <v>1</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>80</v>
+      </c>
       <c r="E11" s="29"/>
       <c r="F11" s="29"/>
       <c r="G11" s="29"/>
@@ -1888,12 +2094,12 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="41"/>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="42"/>
+      <c r="C12" s="44">
         <v>2</v>
       </c>
-      <c r="C12" s="43"/>
       <c r="D12" s="40" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
@@ -1904,12 +2110,12 @@
       <c r="K12" s="29"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A13" s="41"/>
-      <c r="B13" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="43"/>
-      <c r="D13" s="40"/>
+      <c r="C13" s="44">
+        <v>3</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>82</v>
+      </c>
       <c r="E13" s="29"/>
       <c r="F13" s="29"/>
       <c r="G13" s="29"/>
@@ -1922,10 +2128,10 @@
       <c r="A14" s="41"/>
       <c r="B14" s="42"/>
       <c r="C14" s="44">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
@@ -1939,10 +2145,10 @@
       <c r="A15" s="41"/>
       <c r="B15" s="42"/>
       <c r="C15" s="44">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
@@ -1953,11 +2159,13 @@
       <c r="K15" s="29"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C16" s="44">
-        <v>3</v>
-      </c>
-      <c r="D16" s="40" t="s">
-        <v>61</v>
+      <c r="A16" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="49"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51" t="s">
+        <v>10</v>
       </c>
       <c r="E16" s="29"/>
       <c r="F16" s="29"/>
@@ -1967,14 +2175,14 @@
       <c r="J16" s="29"/>
       <c r="K16" s="29"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="41"/>
-      <c r="B17" s="42"/>
-      <c r="C17" s="44">
-        <v>4</v>
-      </c>
+      <c r="B17" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="43"/>
       <c r="D17" s="40" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
@@ -1986,13 +2194,11 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="41"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="44">
-        <v>5</v>
-      </c>
-      <c r="D18" s="40" t="s">
-        <v>63</v>
-      </c>
+      <c r="B18" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="43"/>
+      <c r="D18" s="40"/>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
       <c r="G18" s="29"/>
@@ -2002,11 +2208,13 @@
       <c r="K18" s="29"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C19" s="54">
-        <v>6</v>
-      </c>
-      <c r="D19" s="55" t="s">
-        <v>64</v>
+      <c r="A19" s="41"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="44">
+        <v>1</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>51</v>
       </c>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
@@ -2017,13 +2225,13 @@
       <c r="K19" s="29"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A20" s="48" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="50"/>
-      <c r="D20" s="51" t="s">
-        <v>10</v>
+      <c r="A20" s="41"/>
+      <c r="B20" s="42"/>
+      <c r="C20" s="44">
+        <v>2</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>52</v>
       </c>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
@@ -2033,14 +2241,14 @@
       <c r="J20" s="29"/>
       <c r="K20" s="29"/>
     </row>
-    <row r="21" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="41"/>
-      <c r="B21" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="40" t="s">
-        <v>46</v>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A21" s="30"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="45">
+        <v>3</v>
+      </c>
+      <c r="D21" s="35" t="s">
+        <v>44</v>
       </c>
       <c r="E21" s="29"/>
       <c r="F21" s="29"/>
@@ -2051,12 +2259,13 @@
       <c r="K21" s="29"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A22" s="41"/>
-      <c r="B22" s="42" t="s">
-        <v>9</v>
+      <c r="A22" s="41" t="s">
+        <v>43</v>
       </c>
       <c r="C22" s="43"/>
-      <c r="D22" s="40"/>
+      <c r="D22" s="46" t="s">
+        <v>11</v>
+      </c>
       <c r="E22" s="29"/>
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
@@ -2067,12 +2276,12 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="41"/>
-      <c r="B23" s="42"/>
-      <c r="C23" s="44">
-        <v>1</v>
-      </c>
+      <c r="B23" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="43"/>
       <c r="D23" s="40" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E23" s="29"/>
       <c r="F23" s="29"/>
@@ -2084,13 +2293,11 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="41"/>
-      <c r="B24" s="42"/>
-      <c r="C24" s="44">
-        <v>2</v>
-      </c>
-      <c r="D24" s="40" t="s">
-        <v>52</v>
-      </c>
+      <c r="B24" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="43"/>
+      <c r="D24" s="40"/>
       <c r="E24" s="29"/>
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
@@ -2100,13 +2307,13 @@
       <c r="K24" s="29"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A25" s="30"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="45">
-        <v>3</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>44</v>
+      <c r="A25" s="41"/>
+      <c r="B25" s="42"/>
+      <c r="C25" s="44">
+        <v>1</v>
+      </c>
+      <c r="D25" s="40" t="s">
+        <v>45</v>
       </c>
       <c r="E25" s="29"/>
       <c r="F25" s="29"/>
@@ -2117,12 +2324,13 @@
       <c r="K25" s="29"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="41" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="43"/>
-      <c r="D26" s="46" t="s">
-        <v>11</v>
+      <c r="A26" s="41"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="44">
+        <v>2</v>
+      </c>
+      <c r="D26" s="47" t="s">
+        <v>48</v>
       </c>
       <c r="E26" s="29"/>
       <c r="F26" s="29"/>
@@ -2134,12 +2342,12 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="41"/>
-      <c r="B27" s="42" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" s="43"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="44">
+        <v>3</v>
+      </c>
       <c r="D27" s="40" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
@@ -2150,12 +2358,14 @@
       <c r="K27" s="29"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A28" s="41"/>
-      <c r="B28" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="43"/>
-      <c r="D28" s="40"/>
+      <c r="A28" s="30"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="45">
+        <v>4</v>
+      </c>
+      <c r="D28" s="35" t="s">
+        <v>50</v>
+      </c>
       <c r="E28" s="29"/>
       <c r="F28" s="29"/>
       <c r="G28" s="29"/>
@@ -3169,19 +3379,24 @@
       <c r="K104" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7CFED9-3A2B-4A15-891A-1A195DE19435}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D16BEC-6A93-49D4-A9D0-6AC6792BFE42}">
   <dimension ref="A1:K104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3193,10 +3408,10 @@
   <sheetData>
     <row r="1" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D1" s="56" t="s">
-        <v>74</v>
+        <v>64</v>
+      </c>
+      <c r="D1" s="53" t="s">
+        <v>118</v>
       </c>
       <c r="E1" s="29"/>
       <c r="F1" s="29"/>
@@ -3231,7 +3446,7 @@
       <c r="B4" s="26"/>
       <c r="C4" s="27"/>
       <c r="D4" s="28" t="s">
-        <v>53</v>
+        <v>119</v>
       </c>
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
@@ -3258,14 +3473,14 @@
       <c r="J5" s="29"/>
       <c r="K5" s="29"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A6" s="52" t="s">
+    <row r="6" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="53"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="32"/>
       <c r="D6" s="35" t="s">
-        <v>54</v>
+        <v>120</v>
       </c>
       <c r="E6" s="29"/>
       <c r="F6" s="29"/>
@@ -3282,7 +3497,7 @@
       <c r="B7" s="31"/>
       <c r="C7" s="32"/>
       <c r="D7" s="35" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="E7" s="29"/>
       <c r="F7" s="29"/>
@@ -3299,7 +3514,7 @@
       <c r="B8" s="31"/>
       <c r="C8" s="32"/>
       <c r="D8" s="35" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="E8" s="29"/>
       <c r="F8" s="29"/>
@@ -3316,7 +3531,7 @@
       <c r="B9" s="34"/>
       <c r="C9" s="32"/>
       <c r="D9" s="35" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
@@ -3333,7 +3548,7 @@
       <c r="B10" s="34"/>
       <c r="C10" s="36"/>
       <c r="D10" s="35" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
       <c r="E10" s="29"/>
       <c r="F10" s="29"/>
@@ -3365,7 +3580,7 @@
       </c>
       <c r="C12" s="43"/>
       <c r="D12" s="40" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
       <c r="E12" s="29"/>
       <c r="F12" s="29"/>
@@ -3397,7 +3612,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="40" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
@@ -3414,7 +3629,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>60</v>
+        <v>106</v>
       </c>
       <c r="E15" s="29"/>
       <c r="F15" s="29"/>
@@ -3429,7 +3644,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>61</v>
+        <v>107</v>
       </c>
       <c r="E16" s="29"/>
       <c r="F16" s="29"/>
@@ -3446,7 +3661,7 @@
         <v>4</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>62</v>
+        <v>108</v>
       </c>
       <c r="E17" s="29"/>
       <c r="F17" s="29"/>
@@ -3463,7 +3678,7 @@
         <v>5</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>63</v>
+        <v>109</v>
       </c>
       <c r="E18" s="29"/>
       <c r="F18" s="29"/>
@@ -3474,11 +3689,11 @@
       <c r="K18" s="29"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="C19" s="54">
+      <c r="C19" s="44">
         <v>6</v>
       </c>
-      <c r="D19" s="55" t="s">
-        <v>73</v>
+      <c r="D19" s="52" t="s">
+        <v>111</v>
       </c>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
@@ -3512,7 +3727,7 @@
       </c>
       <c r="C21" s="43"/>
       <c r="D21" s="40" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="E21" s="29"/>
       <c r="F21" s="29"/>
@@ -3540,11 +3755,11 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="41"/>
       <c r="B23" s="42"/>
-      <c r="C23" s="57" t="s">
-        <v>69</v>
+      <c r="C23" s="54" t="s">
+        <v>67</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E23" s="29"/>
       <c r="F23" s="29"/>
@@ -3561,7 +3776,7 @@
         <v>4</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>71</v>
+        <v>115</v>
       </c>
       <c r="E24" s="29"/>
       <c r="F24" s="29"/>
@@ -3572,13 +3787,13 @@
       <c r="K24" s="29"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A25" s="65"/>
-      <c r="B25" s="66"/>
-      <c r="C25" s="67">
+      <c r="A25" s="60"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="62">
         <v>5</v>
       </c>
-      <c r="D25" s="68" t="s">
-        <v>72</v>
+      <c r="D25" s="63" t="s">
+        <v>116</v>
       </c>
       <c r="E25" s="29"/>
       <c r="F25" s="29"/>
@@ -3589,10 +3804,9 @@
       <c r="K25" s="29"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="58"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="61"/>
+      <c r="C26">
+        <v>6</v>
+      </c>
       <c r="E26" s="29"/>
       <c r="F26" s="29"/>
       <c r="G26" s="29"/>
@@ -3602,10 +3816,14 @@
       <c r="K26" s="29"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A27" s="58"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="62"/>
+      <c r="A27" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="51" t="s">
+        <v>11</v>
+      </c>
       <c r="E27" s="29"/>
       <c r="F27" s="29"/>
       <c r="G27" s="29"/>
@@ -3615,10 +3833,14 @@
       <c r="K27" s="29"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A28" s="58"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="62"/>
+      <c r="A28" s="41"/>
+      <c r="B28" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="43"/>
+      <c r="D28" s="40" t="s">
+        <v>113</v>
+      </c>
       <c r="E28" s="29"/>
       <c r="F28" s="29"/>
       <c r="G28" s="29"/>
@@ -3628,10 +3850,12 @@
       <c r="K28" s="29"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A29" s="58"/>
-      <c r="B29" s="58"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="62"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="43"/>
+      <c r="D29" s="40"/>
       <c r="E29" s="29"/>
       <c r="F29" s="29"/>
       <c r="G29" s="29"/>
@@ -3641,10 +3865,14 @@
       <c r="K29" s="29"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A30" s="58"/>
-      <c r="B30" s="58"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="64"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="D30" s="40" t="s">
+        <v>68</v>
+      </c>
       <c r="E30" s="29"/>
       <c r="F30" s="29"/>
       <c r="G30" s="29"/>
@@ -3654,10 +3882,14 @@
       <c r="K30" s="29"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A31" s="58"/>
-      <c r="B31" s="58"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="62"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="44">
+        <v>4</v>
+      </c>
+      <c r="D31" s="40" t="s">
+        <v>114</v>
+      </c>
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
       <c r="G31" s="29"/>
@@ -3667,10 +3899,14 @@
       <c r="K31" s="29"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A32" s="58"/>
-      <c r="B32" s="58"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="62"/>
+      <c r="A32" s="60"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="62">
+        <v>5</v>
+      </c>
+      <c r="D32" s="63" t="s">
+        <v>117</v>
+      </c>
       <c r="E32" s="29"/>
       <c r="F32" s="29"/>
       <c r="G32" s="29"/>
@@ -4621,4 +4857,1705 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C7CFED9-3A2B-4A15-891A-1A195DE19435}">
+  <dimension ref="A1:K104"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.59765625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15.1328125" customWidth="1"/>
+    <col min="3" max="3" width="6" customWidth="1"/>
+    <col min="4" max="4" width="75.3984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="70.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="53" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A5" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="33">
+        <v>0</v>
+      </c>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="65"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="34"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="34"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" s="41"/>
+      <c r="B12" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="43"/>
+      <c r="D12" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" s="41"/>
+      <c r="B13" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="43"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" s="41"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="44">
+        <v>1</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" s="41"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="44">
+        <v>2</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C16" s="44">
+        <v>3</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>61</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A17" s="41"/>
+      <c r="B17" s="42"/>
+      <c r="C17" s="44">
+        <v>4</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A18" s="41"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="44">
+        <v>5</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="C19" s="44">
+        <v>6</v>
+      </c>
+      <c r="D19" s="52" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A20" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="49"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A21" s="41"/>
+      <c r="B21" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="43"/>
+      <c r="D21" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A22" s="41"/>
+      <c r="B22" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="43"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A23" s="41"/>
+      <c r="B23" s="42"/>
+      <c r="C23" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A24" s="41"/>
+      <c r="B24" s="42"/>
+      <c r="C24" s="44">
+        <v>4</v>
+      </c>
+      <c r="D24" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A25" s="60"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="62">
+        <v>5</v>
+      </c>
+      <c r="D25" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26" s="42"/>
+      <c r="C26" s="55"/>
+      <c r="D26" s="56"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A27" s="42"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="57"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A28" s="42"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="55"/>
+      <c r="D28" s="57"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" s="42"/>
+      <c r="B29" s="42"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" s="42"/>
+      <c r="B30" s="42"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A31" s="42"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A32" s="42"/>
+      <c r="B32" s="42"/>
+      <c r="C32" s="58"/>
+      <c r="D32" s="57"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A33" s="29"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A34" s="29"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A35" s="29"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A36" s="29"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A37" s="29"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A38" s="29"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A39" s="29"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="29"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A40" s="29"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A41" s="29"/>
+      <c r="B41" s="29"/>
+      <c r="C41" s="29"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="29"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A42" s="29"/>
+      <c r="B42" s="29"/>
+      <c r="C42" s="29"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A43" s="29"/>
+      <c r="B43" s="29"/>
+      <c r="C43" s="29"/>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
+      <c r="C44" s="29"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A45" s="29"/>
+      <c r="B45" s="29"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="29"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A46" s="29"/>
+      <c r="B46" s="29"/>
+      <c r="C46" s="29"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
+      <c r="K46" s="29"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A47" s="29"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
+      <c r="K47" s="29"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A48" s="29"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="29"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="29"/>
+      <c r="K48" s="29"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A49" s="29"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="29"/>
+      <c r="K49" s="29"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A50" s="29"/>
+      <c r="B50" s="29"/>
+      <c r="C50" s="29"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="29"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A51" s="29"/>
+      <c r="B51" s="29"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="29"/>
+      <c r="K51" s="29"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A52" s="29"/>
+      <c r="B52" s="29"/>
+      <c r="C52" s="29"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="29"/>
+      <c r="G52" s="29"/>
+      <c r="H52" s="29"/>
+      <c r="I52" s="29"/>
+      <c r="J52" s="29"/>
+      <c r="K52" s="29"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A53" s="29"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="29"/>
+      <c r="K53" s="29"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A54" s="29"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="29"/>
+      <c r="I54" s="29"/>
+      <c r="J54" s="29"/>
+      <c r="K54" s="29"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A55" s="29"/>
+      <c r="B55" s="29"/>
+      <c r="C55" s="29"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
+      <c r="J55" s="29"/>
+      <c r="K55" s="29"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A56" s="29"/>
+      <c r="B56" s="29"/>
+      <c r="C56" s="29"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="29"/>
+      <c r="G56" s="29"/>
+      <c r="H56" s="29"/>
+      <c r="I56" s="29"/>
+      <c r="J56" s="29"/>
+      <c r="K56" s="29"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A57" s="29"/>
+      <c r="B57" s="29"/>
+      <c r="C57" s="29"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="29"/>
+      <c r="H57" s="29"/>
+      <c r="I57" s="29"/>
+      <c r="J57" s="29"/>
+      <c r="K57" s="29"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A58" s="29"/>
+      <c r="B58" s="29"/>
+      <c r="C58" s="29"/>
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29"/>
+      <c r="G58" s="29"/>
+      <c r="H58" s="29"/>
+      <c r="I58" s="29"/>
+      <c r="J58" s="29"/>
+      <c r="K58" s="29"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A59" s="29"/>
+      <c r="B59" s="29"/>
+      <c r="C59" s="29"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="29"/>
+      <c r="G59" s="29"/>
+      <c r="H59" s="29"/>
+      <c r="I59" s="29"/>
+      <c r="J59" s="29"/>
+      <c r="K59" s="29"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A60" s="29"/>
+      <c r="B60" s="29"/>
+      <c r="C60" s="29"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
+      <c r="G60" s="29"/>
+      <c r="H60" s="29"/>
+      <c r="I60" s="29"/>
+      <c r="J60" s="29"/>
+      <c r="K60" s="29"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A61" s="29"/>
+      <c r="B61" s="29"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="29"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="29"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="29"/>
+      <c r="I61" s="29"/>
+      <c r="J61" s="29"/>
+      <c r="K61" s="29"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A62" s="29"/>
+      <c r="B62" s="29"/>
+      <c r="C62" s="29"/>
+      <c r="D62" s="29"/>
+      <c r="E62" s="29"/>
+      <c r="F62" s="29"/>
+      <c r="G62" s="29"/>
+      <c r="H62" s="29"/>
+      <c r="I62" s="29"/>
+      <c r="J62" s="29"/>
+      <c r="K62" s="29"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A63" s="29"/>
+      <c r="B63" s="29"/>
+      <c r="C63" s="29"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="29"/>
+      <c r="G63" s="29"/>
+      <c r="H63" s="29"/>
+      <c r="I63" s="29"/>
+      <c r="J63" s="29"/>
+      <c r="K63" s="29"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A64" s="29"/>
+      <c r="B64" s="29"/>
+      <c r="C64" s="29"/>
+      <c r="D64" s="29"/>
+      <c r="E64" s="29"/>
+      <c r="F64" s="29"/>
+      <c r="G64" s="29"/>
+      <c r="H64" s="29"/>
+      <c r="I64" s="29"/>
+      <c r="J64" s="29"/>
+      <c r="K64" s="29"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A65" s="29"/>
+      <c r="B65" s="29"/>
+      <c r="C65" s="29"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="29"/>
+      <c r="G65" s="29"/>
+      <c r="H65" s="29"/>
+      <c r="I65" s="29"/>
+      <c r="J65" s="29"/>
+      <c r="K65" s="29"/>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A66" s="29"/>
+      <c r="B66" s="29"/>
+      <c r="C66" s="29"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="29"/>
+      <c r="G66" s="29"/>
+      <c r="H66" s="29"/>
+      <c r="I66" s="29"/>
+      <c r="J66" s="29"/>
+      <c r="K66" s="29"/>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A67" s="29"/>
+      <c r="B67" s="29"/>
+      <c r="C67" s="29"/>
+      <c r="D67" s="29"/>
+      <c r="E67" s="29"/>
+      <c r="F67" s="29"/>
+      <c r="G67" s="29"/>
+      <c r="H67" s="29"/>
+      <c r="I67" s="29"/>
+      <c r="J67" s="29"/>
+      <c r="K67" s="29"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A68" s="29"/>
+      <c r="B68" s="29"/>
+      <c r="C68" s="29"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="29"/>
+      <c r="G68" s="29"/>
+      <c r="H68" s="29"/>
+      <c r="I68" s="29"/>
+      <c r="J68" s="29"/>
+      <c r="K68" s="29"/>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A69" s="29"/>
+      <c r="B69" s="29"/>
+      <c r="C69" s="29"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="29"/>
+      <c r="G69" s="29"/>
+      <c r="H69" s="29"/>
+      <c r="I69" s="29"/>
+      <c r="J69" s="29"/>
+      <c r="K69" s="29"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A70" s="29"/>
+      <c r="B70" s="29"/>
+      <c r="C70" s="29"/>
+      <c r="D70" s="29"/>
+      <c r="E70" s="29"/>
+      <c r="F70" s="29"/>
+      <c r="G70" s="29"/>
+      <c r="H70" s="29"/>
+      <c r="I70" s="29"/>
+      <c r="J70" s="29"/>
+      <c r="K70" s="29"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A71" s="29"/>
+      <c r="B71" s="29"/>
+      <c r="C71" s="29"/>
+      <c r="D71" s="29"/>
+      <c r="E71" s="29"/>
+      <c r="F71" s="29"/>
+      <c r="G71" s="29"/>
+      <c r="H71" s="29"/>
+      <c r="I71" s="29"/>
+      <c r="J71" s="29"/>
+      <c r="K71" s="29"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A72" s="29"/>
+      <c r="B72" s="29"/>
+      <c r="C72" s="29"/>
+      <c r="D72" s="29"/>
+      <c r="E72" s="29"/>
+      <c r="F72" s="29"/>
+      <c r="G72" s="29"/>
+      <c r="H72" s="29"/>
+      <c r="I72" s="29"/>
+      <c r="J72" s="29"/>
+      <c r="K72" s="29"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A73" s="29"/>
+      <c r="B73" s="29"/>
+      <c r="C73" s="29"/>
+      <c r="D73" s="29"/>
+      <c r="E73" s="29"/>
+      <c r="F73" s="29"/>
+      <c r="G73" s="29"/>
+      <c r="H73" s="29"/>
+      <c r="I73" s="29"/>
+      <c r="J73" s="29"/>
+      <c r="K73" s="29"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A74" s="29"/>
+      <c r="B74" s="29"/>
+      <c r="C74" s="29"/>
+      <c r="D74" s="29"/>
+      <c r="E74" s="29"/>
+      <c r="F74" s="29"/>
+      <c r="G74" s="29"/>
+      <c r="H74" s="29"/>
+      <c r="I74" s="29"/>
+      <c r="J74" s="29"/>
+      <c r="K74" s="29"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A75" s="29"/>
+      <c r="B75" s="29"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="29"/>
+      <c r="E75" s="29"/>
+      <c r="F75" s="29"/>
+      <c r="G75" s="29"/>
+      <c r="H75" s="29"/>
+      <c r="I75" s="29"/>
+      <c r="J75" s="29"/>
+      <c r="K75" s="29"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A76" s="29"/>
+      <c r="B76" s="29"/>
+      <c r="C76" s="29"/>
+      <c r="D76" s="29"/>
+      <c r="E76" s="29"/>
+      <c r="F76" s="29"/>
+      <c r="G76" s="29"/>
+      <c r="H76" s="29"/>
+      <c r="I76" s="29"/>
+      <c r="J76" s="29"/>
+      <c r="K76" s="29"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A77" s="29"/>
+      <c r="B77" s="29"/>
+      <c r="C77" s="29"/>
+      <c r="D77" s="29"/>
+      <c r="E77" s="29"/>
+      <c r="F77" s="29"/>
+      <c r="G77" s="29"/>
+      <c r="H77" s="29"/>
+      <c r="I77" s="29"/>
+      <c r="J77" s="29"/>
+      <c r="K77" s="29"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A78" s="29"/>
+      <c r="B78" s="29"/>
+      <c r="C78" s="29"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="29"/>
+      <c r="F78" s="29"/>
+      <c r="G78" s="29"/>
+      <c r="H78" s="29"/>
+      <c r="I78" s="29"/>
+      <c r="J78" s="29"/>
+      <c r="K78" s="29"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A79" s="29"/>
+      <c r="B79" s="29"/>
+      <c r="C79" s="29"/>
+      <c r="D79" s="29"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="29"/>
+      <c r="G79" s="29"/>
+      <c r="H79" s="29"/>
+      <c r="I79" s="29"/>
+      <c r="J79" s="29"/>
+      <c r="K79" s="29"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A80" s="29"/>
+      <c r="B80" s="29"/>
+      <c r="C80" s="29"/>
+      <c r="D80" s="29"/>
+      <c r="E80" s="29"/>
+      <c r="F80" s="29"/>
+      <c r="G80" s="29"/>
+      <c r="H80" s="29"/>
+      <c r="I80" s="29"/>
+      <c r="J80" s="29"/>
+      <c r="K80" s="29"/>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A81" s="29"/>
+      <c r="B81" s="29"/>
+      <c r="C81" s="29"/>
+      <c r="D81" s="29"/>
+      <c r="E81" s="29"/>
+      <c r="F81" s="29"/>
+      <c r="G81" s="29"/>
+      <c r="H81" s="29"/>
+      <c r="I81" s="29"/>
+      <c r="J81" s="29"/>
+      <c r="K81" s="29"/>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A82" s="29"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="29"/>
+      <c r="E82" s="29"/>
+      <c r="F82" s="29"/>
+      <c r="G82" s="29"/>
+      <c r="H82" s="29"/>
+      <c r="I82" s="29"/>
+      <c r="J82" s="29"/>
+      <c r="K82" s="29"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A83" s="29"/>
+      <c r="B83" s="29"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="29"/>
+      <c r="E83" s="29"/>
+      <c r="F83" s="29"/>
+      <c r="G83" s="29"/>
+      <c r="H83" s="29"/>
+      <c r="I83" s="29"/>
+      <c r="J83" s="29"/>
+      <c r="K83" s="29"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A84" s="29"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="29"/>
+      <c r="D84" s="29"/>
+      <c r="E84" s="29"/>
+      <c r="F84" s="29"/>
+      <c r="G84" s="29"/>
+      <c r="H84" s="29"/>
+      <c r="I84" s="29"/>
+      <c r="J84" s="29"/>
+      <c r="K84" s="29"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A85" s="29"/>
+      <c r="B85" s="29"/>
+      <c r="C85" s="29"/>
+      <c r="D85" s="29"/>
+      <c r="E85" s="29"/>
+      <c r="F85" s="29"/>
+      <c r="G85" s="29"/>
+      <c r="H85" s="29"/>
+      <c r="I85" s="29"/>
+      <c r="J85" s="29"/>
+      <c r="K85" s="29"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A86" s="29"/>
+      <c r="B86" s="29"/>
+      <c r="C86" s="29"/>
+      <c r="D86" s="29"/>
+      <c r="E86" s="29"/>
+      <c r="F86" s="29"/>
+      <c r="G86" s="29"/>
+      <c r="H86" s="29"/>
+      <c r="I86" s="29"/>
+      <c r="J86" s="29"/>
+      <c r="K86" s="29"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A87" s="29"/>
+      <c r="B87" s="29"/>
+      <c r="C87" s="29"/>
+      <c r="D87" s="29"/>
+      <c r="E87" s="29"/>
+      <c r="F87" s="29"/>
+      <c r="G87" s="29"/>
+      <c r="H87" s="29"/>
+      <c r="I87" s="29"/>
+      <c r="J87" s="29"/>
+      <c r="K87" s="29"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A88" s="29"/>
+      <c r="B88" s="29"/>
+      <c r="C88" s="29"/>
+      <c r="D88" s="29"/>
+      <c r="E88" s="29"/>
+      <c r="F88" s="29"/>
+      <c r="G88" s="29"/>
+      <c r="H88" s="29"/>
+      <c r="I88" s="29"/>
+      <c r="J88" s="29"/>
+      <c r="K88" s="29"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A89" s="29"/>
+      <c r="B89" s="29"/>
+      <c r="C89" s="29"/>
+      <c r="D89" s="29"/>
+      <c r="E89" s="29"/>
+      <c r="F89" s="29"/>
+      <c r="G89" s="29"/>
+      <c r="H89" s="29"/>
+      <c r="I89" s="29"/>
+      <c r="J89" s="29"/>
+      <c r="K89" s="29"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A90" s="29"/>
+      <c r="B90" s="29"/>
+      <c r="C90" s="29"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
+      <c r="G90" s="29"/>
+      <c r="H90" s="29"/>
+      <c r="I90" s="29"/>
+      <c r="J90" s="29"/>
+      <c r="K90" s="29"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A91" s="29"/>
+      <c r="B91" s="29"/>
+      <c r="C91" s="29"/>
+      <c r="D91" s="29"/>
+      <c r="E91" s="29"/>
+      <c r="F91" s="29"/>
+      <c r="G91" s="29"/>
+      <c r="H91" s="29"/>
+      <c r="I91" s="29"/>
+      <c r="J91" s="29"/>
+      <c r="K91" s="29"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A92" s="29"/>
+      <c r="B92" s="29"/>
+      <c r="C92" s="29"/>
+      <c r="D92" s="29"/>
+      <c r="E92" s="29"/>
+      <c r="F92" s="29"/>
+      <c r="G92" s="29"/>
+      <c r="H92" s="29"/>
+      <c r="I92" s="29"/>
+      <c r="J92" s="29"/>
+      <c r="K92" s="29"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A93" s="29"/>
+      <c r="B93" s="29"/>
+      <c r="C93" s="29"/>
+      <c r="D93" s="29"/>
+      <c r="E93" s="29"/>
+      <c r="F93" s="29"/>
+      <c r="G93" s="29"/>
+      <c r="H93" s="29"/>
+      <c r="I93" s="29"/>
+      <c r="J93" s="29"/>
+      <c r="K93" s="29"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A94" s="29"/>
+      <c r="B94" s="29"/>
+      <c r="C94" s="29"/>
+      <c r="D94" s="29"/>
+      <c r="E94" s="29"/>
+      <c r="F94" s="29"/>
+      <c r="G94" s="29"/>
+      <c r="H94" s="29"/>
+      <c r="I94" s="29"/>
+      <c r="J94" s="29"/>
+      <c r="K94" s="29"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A95" s="29"/>
+      <c r="B95" s="29"/>
+      <c r="C95" s="29"/>
+      <c r="D95" s="29"/>
+      <c r="E95" s="29"/>
+      <c r="F95" s="29"/>
+      <c r="G95" s="29"/>
+      <c r="H95" s="29"/>
+      <c r="I95" s="29"/>
+      <c r="J95" s="29"/>
+      <c r="K95" s="29"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A96" s="29"/>
+      <c r="B96" s="29"/>
+      <c r="C96" s="29"/>
+      <c r="D96" s="29"/>
+      <c r="E96" s="29"/>
+      <c r="F96" s="29"/>
+      <c r="G96" s="29"/>
+      <c r="H96" s="29"/>
+      <c r="I96" s="29"/>
+      <c r="J96" s="29"/>
+      <c r="K96" s="29"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A97" s="29"/>
+      <c r="B97" s="29"/>
+      <c r="C97" s="29"/>
+      <c r="D97" s="29"/>
+      <c r="E97" s="29"/>
+      <c r="F97" s="29"/>
+      <c r="G97" s="29"/>
+      <c r="H97" s="29"/>
+      <c r="I97" s="29"/>
+      <c r="J97" s="29"/>
+      <c r="K97" s="29"/>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A98" s="29"/>
+      <c r="B98" s="29"/>
+      <c r="C98" s="29"/>
+      <c r="D98" s="29"/>
+      <c r="E98" s="29"/>
+      <c r="F98" s="29"/>
+      <c r="G98" s="29"/>
+      <c r="H98" s="29"/>
+      <c r="I98" s="29"/>
+      <c r="J98" s="29"/>
+      <c r="K98" s="29"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A99" s="29"/>
+      <c r="B99" s="29"/>
+      <c r="C99" s="29"/>
+      <c r="D99" s="29"/>
+      <c r="E99" s="29"/>
+      <c r="F99" s="29"/>
+      <c r="G99" s="29"/>
+      <c r="H99" s="29"/>
+      <c r="I99" s="29"/>
+      <c r="J99" s="29"/>
+      <c r="K99" s="29"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A100" s="29"/>
+      <c r="B100" s="29"/>
+      <c r="C100" s="29"/>
+      <c r="D100" s="29"/>
+      <c r="E100" s="29"/>
+      <c r="F100" s="29"/>
+      <c r="G100" s="29"/>
+      <c r="H100" s="29"/>
+      <c r="I100" s="29"/>
+      <c r="J100" s="29"/>
+      <c r="K100" s="29"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A101" s="29"/>
+      <c r="B101" s="29"/>
+      <c r="C101" s="29"/>
+      <c r="D101" s="29"/>
+      <c r="E101" s="29"/>
+      <c r="F101" s="29"/>
+      <c r="G101" s="29"/>
+      <c r="H101" s="29"/>
+      <c r="I101" s="29"/>
+      <c r="J101" s="29"/>
+      <c r="K101" s="29"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A102" s="29"/>
+      <c r="B102" s="29"/>
+      <c r="C102" s="29"/>
+      <c r="D102" s="29"/>
+      <c r="E102" s="29"/>
+      <c r="F102" s="29"/>
+      <c r="G102" s="29"/>
+      <c r="H102" s="29"/>
+      <c r="I102" s="29"/>
+      <c r="J102" s="29"/>
+      <c r="K102" s="29"/>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A103" s="29"/>
+      <c r="B103" s="29"/>
+      <c r="C103" s="29"/>
+      <c r="D103" s="29"/>
+      <c r="E103" s="29"/>
+      <c r="F103" s="29"/>
+      <c r="G103" s="29"/>
+      <c r="H103" s="29"/>
+      <c r="I103" s="29"/>
+      <c r="J103" s="29"/>
+      <c r="K103" s="29"/>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A104" s="29"/>
+      <c r="B104" s="29"/>
+      <c r="C104" s="29"/>
+      <c r="D104" s="29"/>
+      <c r="E104" s="29"/>
+      <c r="F104" s="29"/>
+      <c r="G104" s="29"/>
+      <c r="H104" s="29"/>
+      <c r="I104" s="29"/>
+      <c r="J104" s="29"/>
+      <c r="K104" s="29"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7B31F85-E4F5-4B25-A08E-A898F868D44E}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="6.86328125" customWidth="1"/>
+    <col min="2" max="2" width="5.265625" customWidth="1"/>
+    <col min="3" max="3" width="8.73046875" customWidth="1"/>
+    <col min="4" max="4" width="88.1328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="9"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="19">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C12" s="19">
+        <v>2</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="20">
+        <v>3</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="4"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="71" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="18"/>
+      <c r="D15" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="21">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C18" s="21">
+        <v>2</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="72"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="74">
+        <v>3</v>
+      </c>
+      <c r="D19" s="75" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="4"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="71" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="21">
+        <v>1</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="72"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="74">
+        <v>2</v>
+      </c>
+      <c r="D24" s="75" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="77"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>